<commit_message>
Update Sequence Diagram + Input effort
</commit_message>
<xml_diff>
--- a/1.DELIVERABLE/1.8 TASK_ASSIGN/BSS_TaskAssign.xlsx
+++ b/1.DELIVERABLE/1.8 TASK_ASSIGN/BSS_TaskAssign.xlsx
@@ -1415,7 +1415,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1426,8 +1426,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:O265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G256" sqref="G256"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H249" sqref="H249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9157,8 +9157,12 @@
       <c r="F242" s="24">
         <v>42918</v>
       </c>
-      <c r="G242" s="20"/>
-      <c r="H242" s="20"/>
+      <c r="G242" s="20">
+        <v>7</v>
+      </c>
+      <c r="H242" s="20">
+        <v>6</v>
+      </c>
       <c r="I242" s="24">
         <v>43010</v>
       </c>
@@ -9261,8 +9265,12 @@
       <c r="F246" s="24">
         <v>42918</v>
       </c>
-      <c r="G246" s="20"/>
-      <c r="H246" s="20"/>
+      <c r="G246" s="20">
+        <v>7</v>
+      </c>
+      <c r="H246" s="20">
+        <v>6</v>
+      </c>
       <c r="I246" s="24">
         <v>43010</v>
       </c>
@@ -9391,8 +9399,12 @@
       <c r="F251" s="24">
         <v>42918</v>
       </c>
-      <c r="G251" s="20"/>
-      <c r="H251" s="20"/>
+      <c r="G251" s="20">
+        <v>7</v>
+      </c>
+      <c r="H251" s="20">
+        <v>8</v>
+      </c>
       <c r="I251" s="24">
         <v>43010</v>
       </c>

</xml_diff>